<commit_message>
test sever use excel data and pytest setup local ser
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HE\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2272CB-B77F-458A-B55D-442CFD35FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AE3FEF-8202-4311-A51B-56B3032198CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="6648" windowWidth="34560" windowHeight="18552" xr2:uid="{80D4BAB8-107E-43D2-A685-1FAF29E147C3}"/>
+    <workbookView xWindow="8352" yWindow="11856" windowWidth="34560" windowHeight="18552" activeTab="1" xr2:uid="{80D4BAB8-107E-43D2-A685-1FAF29E147C3}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="serlogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +64,78 @@
   </si>
   <si>
     <t>root</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://192.168.31.70:5000/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"username": "user1", "password": "password1"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"username": "user1", "password": "password"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"username": "user1"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少用户名或密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"password": "password"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expected</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"message": "登录成功"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"message": "用户名或密码错误"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"message": "缺少用户名或密码"}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -70,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +154,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -104,18 +186,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950DA25F-48F4-4C9A-8CFE-43657A3AC005}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -472,4 +561,133 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A95348E-2261-40E0-9644-3DB563971C61}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A9BB0D93-4B2F-4712-84DA-715C174EFC22}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{64564478-9E04-4498-A585-AE4F0EFAB9ED}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{7AE420AA-CC51-408A-B2EB-D0BDAC3E3CB0}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{D769C8A2-02C8-42AB-AFBC-A3057EEC5542}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>